<commit_message>
Remove yellow pixel in figure
</commit_message>
<xml_diff>
--- a/figures/resources/pixels.xlsx
+++ b/figures/resources/pixels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tischer/Documents/training-resources/figures/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF4F8FE-8341-A940-8BCC-3E66FBB22D76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE6744F-6D20-0F40-ADB1-1FF330FA3A59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{AFB592CA-EABC-C547-8EDD-0658AD58DA5C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{AFB592CA-EABC-C547-8EDD-0658AD58DA5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -113,9 +113,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -434,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55615056-DDA6-7547-9E31-DDAB8BE0B80D}">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="D1" zoomScale="86" zoomScaleNormal="100" zoomScalePageLayoutView="86" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScale="86" zoomScaleNormal="100" zoomScalePageLayoutView="86" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5" defaultRowHeight="21.5" customHeight="1"/>
@@ -792,7 +789,7 @@
       <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>2</v>
       </c>
       <c r="E6" s="5">

</xml_diff>

<commit_message>
added exercise for EM and padding details
</commit_message>
<xml_diff>
--- a/figures/resources/pixels.xlsx
+++ b/figures/resources/pixels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tischer/Documents/training-resources/figures/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akhan\training-resources\figures\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE6744F-6D20-0F40-ADB1-1FF330FA3A59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162D4E27-429C-4835-A4F0-C0D0D190517F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{AFB592CA-EABC-C547-8EDD-0658AD58DA5C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{AFB592CA-EABC-C547-8EDD-0658AD58DA5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -52,6 +52,18 @@
       <color rgb="FF00B050"/>
       <name val="Courier"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -114,6 +126,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,19 +447,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55615056-DDA6-7547-9E31-DDAB8BE0B80D}">
-  <dimension ref="A1:AA22"/>
+  <dimension ref="A1:AK22"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScale="86" zoomScaleNormal="100" zoomScalePageLayoutView="86" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="AJ9" sqref="AJ9:AK9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.5" defaultRowHeight="21.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="21.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.5" style="1"/>
     <col min="2" max="16384" width="3.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" ht="21.5" customHeight="1">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="4">
         <v>0</v>
@@ -507,7 +525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="21.5" customHeight="1">
+    <row r="2" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -575,7 +593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="21.5" customHeight="1">
+    <row r="3" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -643,7 +661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="21.5" customHeight="1">
+    <row r="4" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -711,7 +729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="21.5" customHeight="1">
+    <row r="5" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -778,8 +796,23 @@
       <c r="V5" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" ht="21.5" customHeight="1">
+      <c r="AG5" s="6">
+        <v>48</v>
+      </c>
+      <c r="AH5" s="6">
+        <v>65</v>
+      </c>
+      <c r="AI5" s="6">
+        <v>57</v>
+      </c>
+      <c r="AJ5" s="6">
+        <v>63</v>
+      </c>
+      <c r="AK5" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -846,8 +879,23 @@
       <c r="V6" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" ht="21.5" customHeight="1">
+      <c r="AG6" s="6">
+        <v>56</v>
+      </c>
+      <c r="AH6" s="6">
+        <v>73</v>
+      </c>
+      <c r="AI6" s="6">
+        <v>61</v>
+      </c>
+      <c r="AJ6" s="6">
+        <v>60</v>
+      </c>
+      <c r="AK6" s="6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -914,8 +962,23 @@
       <c r="V7" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" ht="21.5" customHeight="1">
+      <c r="AG7" s="6">
+        <v>46</v>
+      </c>
+      <c r="AH7" s="6">
+        <v>56</v>
+      </c>
+      <c r="AI7" s="7">
+        <v>57</v>
+      </c>
+      <c r="AJ7" s="6">
+        <v>61</v>
+      </c>
+      <c r="AK7" s="6">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -982,8 +1045,23 @@
       <c r="V8" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" ht="21.5" customHeight="1">
+      <c r="AG8" s="6">
+        <v>54</v>
+      </c>
+      <c r="AH8" s="6">
+        <v>55</v>
+      </c>
+      <c r="AI8" s="6">
+        <v>58</v>
+      </c>
+      <c r="AJ8" s="6">
+        <v>80</v>
+      </c>
+      <c r="AK8" s="6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1051,8 +1129,23 @@
         <v>1</v>
       </c>
       <c r="AA9" s="3"/>
-    </row>
-    <row r="10" spans="1:27" ht="21.5" customHeight="1">
+      <c r="AG9" s="6">
+        <v>45</v>
+      </c>
+      <c r="AH9" s="6">
+        <v>68</v>
+      </c>
+      <c r="AI9" s="6">
+        <v>73</v>
+      </c>
+      <c r="AJ9" s="6">
+        <v>74</v>
+      </c>
+      <c r="AK9" s="6">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1120,7 +1213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="21.5" customHeight="1">
+    <row r="11" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1188,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="21.5" customHeight="1">
+    <row r="12" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1256,7 +1349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="21.5" customHeight="1">
+    <row r="13" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1324,7 +1417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="21.5" customHeight="1">
+    <row r="14" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1392,7 +1485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="21.5" customHeight="1">
+    <row r="15" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1460,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="21.5" customHeight="1">
+    <row r="16" spans="1:37" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1528,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="21.5" customHeight="1">
+    <row r="17" spans="1:22" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -1596,7 +1689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="21.5" customHeight="1">
+    <row r="18" spans="1:22" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -1664,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="21.5" customHeight="1">
+    <row r="19" spans="1:22" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -1732,7 +1825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="21.5" customHeight="1">
+    <row r="20" spans="1:22" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -1800,7 +1893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="21.5" customHeight="1">
+    <row r="21" spans="1:22" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -1868,7 +1961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="21.5" customHeight="1">
+    <row r="22" spans="1:22" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -1938,6 +2031,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>